<commit_message>
Ahora de verdad excels bien
</commit_message>
<xml_diff>
--- a/Datos/CLIENTE.xlsx
+++ b/Datos/CLIENTE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Desktop\UNIVERSIDAD\TERCERO\2_Administración-bases-de-datos\Trabajo-grupo\Datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diego\Desktop\Projecto_ABD\ABD\Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E73B8A0-A082-4A18-A4B6-DC0D8B40B1F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EB48249-C5AB-4486-AA38-D660B0A5E9F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="2595" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -114,10 +114,10 @@
     <t>C/ CallejónDiagón, nº 12</t>
   </si>
   <si>
-    <t>2375 Pennsylvania Av. NW, 20037 Washington DC</t>
-  </si>
-  <si>
     <t>Callejón Pereza Buscar Datos</t>
+  </si>
+  <si>
+    <t>Av. NW, 20037 Washington</t>
   </si>
 </sst>
 </file>
@@ -443,7 +443,7 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -569,7 +569,7 @@
         <v>39588</v>
       </c>
       <c r="G4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H4" t="s">
         <v>24</v>
@@ -627,7 +627,7 @@
         <v>41311</v>
       </c>
       <c r="G6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H6" t="s">
         <v>21</v>

</xml_diff>